<commit_message>
Write up sched + assignment handouts
</commit_message>
<xml_diff>
--- a/536CourseSchedule.xlsx
+++ b/536CourseSchedule.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bjboh\Documents\GitHub\pl-course\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bbohrer\Dropbox\PC\Documents\GitHub\pl-course\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D35808B7-B5B9-4016-B5A6-9B8EAE2633C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF38032-EDD1-41BF-8569-D763004D6447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16470" yWindow="405" windowWidth="11985" windowHeight="13425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="4536" sheetId="2" r:id="rId1"/>
+    <sheet name="536" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="93">
   <si>
     <t>Date</t>
   </si>
@@ -262,6 +263,48 @@
   </si>
   <si>
     <t>Final</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>Rust 1: Setup + Vocab</t>
+  </si>
+  <si>
+    <t>Rust 2: Syntax Trees</t>
+  </si>
+  <si>
+    <t>Rust 3: Interpreters</t>
+  </si>
+  <si>
+    <t>Operational Semantics</t>
+  </si>
+  <si>
+    <t>Types</t>
+  </si>
+  <si>
+    <t>Critical Code Studies</t>
+  </si>
+  <si>
+    <t>Visual Arts</t>
+  </si>
+  <si>
+    <t>Interactive Fiction</t>
+  </si>
+  <si>
+    <t>https://pubmed.ncbi.nlm.nih.gov/16204405/</t>
   </si>
 </sst>
 </file>
@@ -590,11 +633,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8144DEB0-8C38-452D-8D42-359E137E414A}">
   <dimension ref="A1:P87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1123,6 +1166,404 @@
     </row>
   </sheetData>
   <hyperlinks>
+    <hyperlink ref="H30" r:id="rId1" xr:uid="{A8010578-CFBC-485F-B48A-37BB2FC2A835}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P87"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="42.7109375" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" t="s">
+        <v>3</v>
+      </c>
+      <c r="P1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1">
+        <v>45163</v>
+      </c>
+      <c r="P2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="1">
+        <v>45167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1">
+        <v>45170</v>
+      </c>
+      <c r="D5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="1">
+        <v>45174</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" s="1">
+        <v>45177</v>
+      </c>
+      <c r="D8" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" s="1">
+        <v>45181</v>
+      </c>
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C11" s="1">
+        <v>45184</v>
+      </c>
+      <c r="D11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" s="1">
+        <v>45188</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>9</v>
+      </c>
+      <c r="B15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C15" s="1">
+        <v>45195</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="1">
+        <v>45198</v>
+      </c>
+      <c r="D16" t="s">
+        <v>82</v>
+      </c>
+      <c r="E16" t="s">
+        <v>19</v>
+      </c>
+      <c r="P16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="1">
+        <v>45202</v>
+      </c>
+      <c r="E18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>12</v>
+      </c>
+      <c r="B19" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" s="1">
+        <v>45205</v>
+      </c>
+      <c r="E19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>13</v>
+      </c>
+      <c r="B21" t="s">
+        <v>90</v>
+      </c>
+      <c r="C21" s="1">
+        <v>45209</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>14</v>
+      </c>
+      <c r="B22" t="s">
+        <v>91</v>
+      </c>
+      <c r="C22" s="1">
+        <v>45212</v>
+      </c>
+      <c r="D22" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C24" s="1"/>
+      <c r="P24" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C25" s="1"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C28" s="1"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C30" s="1"/>
+      <c r="H30" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C32" s="1"/>
+      <c r="H32" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C33" s="1"/>
+      <c r="H33" t="s">
+        <v>37</v>
+      </c>
+      <c r="P33" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C35" s="1"/>
+      <c r="H35" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="L36" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C37" s="1"/>
+      <c r="H37" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="38" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C38" s="1"/>
+      <c r="H38" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C40" s="1"/>
+      <c r="H40" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C41" s="1"/>
+      <c r="H41" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C43" s="1"/>
+      <c r="P43" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="44" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C44" s="1"/>
+      <c r="P44" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B78" s="1"/>
+      <c r="C78" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B79" s="1"/>
+      <c r="C79" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C80" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="81" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C81" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="82" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C82" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="83" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C83" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="84" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C84" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="85" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C85" t="s">
+        <v>47</v>
+      </c>
+      <c r="G85" t="s">
+        <v>57</v>
+      </c>
+      <c r="I85" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="86" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C86" t="s">
+        <v>48</v>
+      </c>
+      <c r="G86" t="s">
+        <v>57</v>
+      </c>
+      <c r="H86" t="s">
+        <v>8</v>
+      </c>
+      <c r="I86" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="87" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C87" t="s">
+        <v>51</v>
+      </c>
+      <c r="G87" t="s">
+        <v>57</v>
+      </c>
+      <c r="I87" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
     <hyperlink ref="H30" r:id="rId1" xr:uid="{BBAC7FC1-2112-450B-BAEB-2BE025889A2F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>